<commit_message>
Aggiunto app.py e requirements.txt
</commit_message>
<xml_diff>
--- a/appuntamenti.xlsx
+++ b/appuntamenti.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,39 @@
       </c>
       <c r="G2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Annamaria</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Luciallo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3398086074</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Terapia</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>